<commit_message>
update: general models, NASDAQ:NET added, Universe file added
</commit_message>
<xml_diff>
--- a/Models/F.xlsx
+++ b/Models/F.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/36a87f973740ffce/Documents/Personal/Models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/36a87f973740ffce/Documents/Personal/Finance/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_D374B8D4A2CB7B54E38FE5D4CED3B8255F7CD40D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_D374B8D4A2CB7B54E38FE5D4CED3B8255F7CD40D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92D0FE91-6CFD-8849-B043-7FCC8EF27263}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="860" windowWidth="33040" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,12 +71,34 @@
     <t xml:space="preserve">Ford Pro </t>
   </si>
   <si>
+    <t>Ford Next</t>
+  </si>
+  <si>
+    <t>investments in new initiatives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ford Credit </t>
+  </si>
+  <si>
+    <t>vehicle-related financing and leasing activities</t>
+  </si>
+  <si>
+    <t>In 2024, we sold approximately 4,470,000 vehicles at wholesale throughout the world.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicles Sold </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hybrid </t>
+  </si>
+  <si>
+    <t>ICV</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial, sans-serif"/>
-      </rPr>
       <t>commercial&amp;gov</t>
     </r>
     <r>
@@ -84,7 +106,8 @@
         <b/>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Arial, sans-serif"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: </t>
     </r>
@@ -92,37 +115,11 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FF000000"/>
-        <rFont val="Arial, sans-serif"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Ford and Lincoln vehicles, service parts, accessories, and services</t>
     </r>
-  </si>
-  <si>
-    <t>Ford Next</t>
-  </si>
-  <si>
-    <t>investments in new initiatives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ford Credit </t>
-  </si>
-  <si>
-    <t>vehicle-related financing and leasing activities</t>
-  </si>
-  <si>
-    <t>In 2024, we sold approximately 4,470,000 vehicles at wholesale throughout the world.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vehicles Sold </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hybrid </t>
-  </si>
-  <si>
-    <t>ICV</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -132,26 +129,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -162,14 +144,23 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial, sans-serif"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial, sans-serif"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -198,15 +189,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -222,6 +215,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -427,177 +424,183 @@
   </sheetPr>
   <dimension ref="B2:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="4"/>
+    <col min="2" max="2" width="16" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="12.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="2" t="s">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("GOOGLEFINANCE(""F"") "),10.43)</f>
+      <c r="C3" s="5">
+        <f>10.43</f>
         <v>10.43</v>
       </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="2" t="s">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4">
-        <v>3892</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="2" t="s">
+      <c r="C4" s="9">
+        <f>3905.696769+70.852</f>
+        <v>3976.548769</v>
+      </c>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4">
-        <f ca="1">C3*C4</f>
-        <v>40593.56</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="2" t="s">
+      <c r="C5" s="6">
+        <f>C3*C4</f>
+        <v>41475.403660669996</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4">
-        <f>13663+14707+9272+706</f>
-        <v>38348</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="2" t="s">
+      <c r="C6" s="6">
+        <f>14362+20864</f>
+        <v>35226</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4">
-        <v>84675</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="2" t="s">
+      <c r="C7" s="6">
+        <f>4286+50154+16644+84186</f>
+        <v>155270</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4">
-        <f ca="1">C5-C6+C7</f>
-        <v>86920.56</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3">
-      <c r="B11" s="5" t="s">
+      <c r="C8" s="6">
+        <f>C5-C6+C7</f>
+        <v>161519.40366066998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
-      <c r="B12" s="5" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:3">
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="6" t="s">
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="6" t="s">
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="6" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B20" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="5">
+      <c r="C20" s="7">
         <v>2023</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="7">
         <v>2024</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="5" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="6">
         <f>72608+99928</f>
         <v>172536</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="6">
         <f>97865+68990</f>
         <v>166855</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="6">
         <f>133743+146249</f>
         <v>279992</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="6">
         <f>187426+215735</f>
         <v>403161</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="6">
         <f>1789561+1850448</f>
         <v>3640009</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="6">
         <f>1793541+1914862</f>
         <v>3708403</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="6">
         <f t="shared" ref="C24:D24" si="0">SUM(C21:C23)</f>
         <v>4092537</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="6">
         <f t="shared" si="0"/>
         <v>4278419</v>
       </c>

</xml_diff>